<commit_message>
update du pla d'adressage cisco
</commit_message>
<xml_diff>
--- a/planAdressage.xlsx
+++ b/planAdressage.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sulie\OneDrive\Documents\Cours_B1\infra-si\infra_si\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sulie\OneDrive\Documents\Cours_B1\infrav2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C593B5DA-9808-405A-9F62-3B08DCF7AF8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A8934F-21C0-48DC-BE82-B68E744482C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="75">
   <si>
     <t>Nombres élèves</t>
   </si>
@@ -158,9 +158,6 @@
     <t>192.168.4.0/29</t>
   </si>
   <si>
-    <t>192.168.5.0/28</t>
-  </si>
-  <si>
     <t>192.168.6.0/30</t>
   </si>
   <si>
@@ -239,12 +236,6 @@
     <t>192.168.5.1</t>
   </si>
   <si>
-    <t>192.168.5.14</t>
-  </si>
-  <si>
-    <t>192.168.5.15</t>
-  </si>
-  <si>
     <t>Serveur</t>
   </si>
   <si>
@@ -258,6 +249,18 @@
   </si>
   <si>
     <t>192.168.20.0/29</t>
+  </si>
+  <si>
+    <t>192.168.5.0/27</t>
+  </si>
+  <si>
+    <t>255.255.255.224</t>
+  </si>
+  <si>
+    <t>192.168.5.27</t>
+  </si>
+  <si>
+    <t>192.168.5.28</t>
   </si>
 </sst>
 </file>
@@ -733,25 +736,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="79" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="69" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" customWidth="1"/>
-    <col min="3" max="3" width="41.140625" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="32.44140625" customWidth="1"/>
+    <col min="3" max="3" width="41.109375" customWidth="1"/>
+    <col min="4" max="4" width="34.33203125" customWidth="1"/>
+    <col min="5" max="5" width="29.109375" customWidth="1"/>
     <col min="6" max="6" width="35" customWidth="1"/>
-    <col min="7" max="7" width="27.140625" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" customWidth="1"/>
-    <col min="10" max="10" width="40.140625" customWidth="1"/>
+    <col min="7" max="7" width="27.109375" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" customWidth="1"/>
+    <col min="9" max="9" width="19.88671875" customWidth="1"/>
+    <col min="10" max="10" width="40.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -768,7 +771,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>600</v>
       </c>
@@ -785,7 +788,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -811,7 +814,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -837,7 +840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -863,7 +866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -889,7 +892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -915,7 +918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -941,7 +944,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -967,7 +970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -993,7 +996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -1019,7 +1022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1045,7 +1048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -1071,7 +1074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -1097,7 +1100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
@@ -1123,7 +1126,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B17">
         <f>B5+B6+B7+B9+B10+B11+B12+B13+B14+B15+B16</f>
         <v>50</v>
@@ -1133,7 +1136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
         <v>23</v>
       </c>
@@ -1153,7 +1156,7 @@
         <v>30</v>
       </c>
       <c r="H18" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I18" t="s">
         <v>31</v>
@@ -1162,7 +1165,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1200,7 +1203,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1217,151 +1220,151 @@
         <v>39</v>
       </c>
       <c r="F20" t="s">
+        <v>71</v>
+      </c>
+      <c r="G20" t="s">
         <v>40</v>
       </c>
-      <c r="G20" t="s">
-        <v>41</v>
-      </c>
       <c r="H20" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>33</v>
       </c>
       <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
         <v>42</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>43</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>44</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
+        <v>72</v>
+      </c>
+      <c r="G21" t="s">
         <v>45</v>
       </c>
-      <c r="F21" t="s">
+      <c r="H21" t="s">
         <v>44</v>
-      </c>
-      <c r="G21" t="s">
-        <v>46</v>
-      </c>
-      <c r="H21" t="s">
-        <v>45</v>
       </c>
       <c r="J21" s="12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" t="s">
+        <v>59</v>
+      </c>
+      <c r="F22" t="s">
+        <v>65</v>
+      </c>
+      <c r="G22" t="s">
+        <v>62</v>
+      </c>
+      <c r="H22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>47</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>52</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>55</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>57</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E23" t="s">
         <v>60</v>
       </c>
-      <c r="F22" t="s">
-        <v>66</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="F23" t="s">
+        <v>73</v>
+      </c>
+      <c r="G23" t="s">
         <v>63</v>
       </c>
-      <c r="H22" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="H23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>48</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>53</v>
       </c>
-      <c r="C23" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="C24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" t="s">
         <v>58</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E24" t="s">
         <v>61</v>
       </c>
-      <c r="F23" t="s">
-        <v>67</v>
-      </c>
-      <c r="G23" t="s">
+      <c r="F24" t="s">
+        <v>74</v>
+      </c>
+      <c r="G24" t="s">
         <v>64</v>
       </c>
-      <c r="H23" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="H24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>49</v>
       </c>
-      <c r="B24" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" t="s">
-        <v>56</v>
-      </c>
-      <c r="D24" t="s">
-        <v>59</v>
-      </c>
-      <c r="E24" t="s">
-        <v>62</v>
-      </c>
-      <c r="F24" t="s">
-        <v>68</v>
-      </c>
-      <c r="G24" t="s">
-        <v>65</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="B25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="G25" t="s">
+        <v>45</v>
+      </c>
+      <c r="H25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>50</v>
-      </c>
-      <c r="B25" t="s">
-        <v>42</v>
-      </c>
-      <c r="C25" t="s">
-        <v>43</v>
-      </c>
-      <c r="D25" t="s">
-        <v>44</v>
-      </c>
-      <c r="E25" t="s">
-        <v>45</v>
-      </c>
-      <c r="F25" t="s">
-        <v>44</v>
-      </c>
-      <c r="G25" t="s">
-        <v>46</v>
-      </c>
-      <c r="H25" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>51</v>
       </c>
       <c r="B26">
         <v>126</v>
@@ -1376,7 +1379,7 @@
         <v>6</v>
       </c>
       <c r="F26">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="G26">
         <v>2</v>
@@ -1385,7 +1388,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="19.2" x14ac:dyDescent="0.45">
       <c r="C27" s="13"/>
     </row>
   </sheetData>

</xml_diff>